<commit_message>
Basic Bay 2 operation working.
</commit_message>
<xml_diff>
--- a/rack_v2.0/PLC/type_B2/data/global_variable_template.xlsx
+++ b/rack_v2.0/PLC/type_B2/data/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="10500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="10500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="966">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -5872,8 +5872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5954,13 +5954,13 @@
         <v>137</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
       </c>
       <c r="F4" t="s">
         <v>133</v>
@@ -6425,7 +6425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F220" sqref="F220"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Operation paused due to management decision.
</commit_message>
<xml_diff>
--- a/rack_v2.0/PLC/type_B2/data/global_variable_template.xlsx
+++ b/rack_v2.0/PLC/type_B2/data/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="10500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="10500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="994">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2935,6 +2935,90 @@
   </si>
   <si>
     <t>D4755</t>
+  </si>
+  <si>
+    <t>D5120</t>
+  </si>
+  <si>
+    <t>D5134</t>
+  </si>
+  <si>
+    <t>D5148</t>
+  </si>
+  <si>
+    <t>D5162</t>
+  </si>
+  <si>
+    <t>D5176</t>
+  </si>
+  <si>
+    <t>D5190</t>
+  </si>
+  <si>
+    <t>D5204</t>
+  </si>
+  <si>
+    <t>D5218</t>
+  </si>
+  <si>
+    <t>D5232</t>
+  </si>
+  <si>
+    <t>D5246</t>
+  </si>
+  <si>
+    <t>D5260</t>
+  </si>
+  <si>
+    <t>D5274</t>
+  </si>
+  <si>
+    <t>D5288</t>
+  </si>
+  <si>
+    <t>D5302</t>
+  </si>
+  <si>
+    <t>REF_PVLookup2_1_Arr</t>
+  </si>
+  <si>
+    <t>REF_PVLookup2_2_Arr</t>
+  </si>
+  <si>
+    <t>REF_PVLookup2_3_Arr</t>
+  </si>
+  <si>
+    <t>REF_PVLookup2_4_Arr</t>
+  </si>
+  <si>
+    <t>REF_PVLookup2_5_Arr</t>
+  </si>
+  <si>
+    <t>REF_PVLookup2_6_Arr</t>
+  </si>
+  <si>
+    <t>REF_PVLookup2_7_Arr</t>
+  </si>
+  <si>
+    <t>REF_PVLookup2_8_Arr</t>
+  </si>
+  <si>
+    <t>REF_PVLookup2_9_Arr</t>
+  </si>
+  <si>
+    <t>REF_PVLookup2_10_Arr</t>
+  </si>
+  <si>
+    <t>REF_PVLookup2_11_Arr</t>
+  </si>
+  <si>
+    <t>REF_PVLookup2_12_Arr</t>
+  </si>
+  <si>
+    <t>REF_PVLookup2_13_Arr</t>
+  </si>
+  <si>
+    <t>REF_PVLookup2_14_Arr</t>
   </si>
 </sst>
 </file>
@@ -5872,7 +5956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+    <sheetView topLeftCell="B2" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -6423,10 +6507,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G219"/>
+  <dimension ref="A1:G233"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F220" sqref="F220"/>
+    <sheetView tabSelected="1" topLeftCell="A198" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C236" sqref="C236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10375,6 +10459,244 @@
       </c>
       <c r="F219" t="s">
         <v>773</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>980</v>
+      </c>
+      <c r="B220" t="s">
+        <v>966</v>
+      </c>
+      <c r="C220" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="D220" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="F220" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>981</v>
+      </c>
+      <c r="B221" t="s">
+        <v>967</v>
+      </c>
+      <c r="C221" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="D221" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="F221" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>982</v>
+      </c>
+      <c r="B222" t="s">
+        <v>968</v>
+      </c>
+      <c r="C222" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="D222" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="F222" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>983</v>
+      </c>
+      <c r="B223" t="s">
+        <v>969</v>
+      </c>
+      <c r="C223" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="D223" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="F223" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>984</v>
+      </c>
+      <c r="B224" t="s">
+        <v>970</v>
+      </c>
+      <c r="C224" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="D224" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="F224" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>985</v>
+      </c>
+      <c r="B225" t="s">
+        <v>971</v>
+      </c>
+      <c r="C225" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="D225" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="F225" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>986</v>
+      </c>
+      <c r="B226" t="s">
+        <v>972</v>
+      </c>
+      <c r="C226" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="D226" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="F226" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>987</v>
+      </c>
+      <c r="B227" t="s">
+        <v>973</v>
+      </c>
+      <c r="C227" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="D227" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="F227" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>988</v>
+      </c>
+      <c r="B228" t="s">
+        <v>974</v>
+      </c>
+      <c r="C228" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="D228" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="F228" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>989</v>
+      </c>
+      <c r="B229" t="s">
+        <v>975</v>
+      </c>
+      <c r="C229" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="D229" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="F229" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>990</v>
+      </c>
+      <c r="B230" t="s">
+        <v>976</v>
+      </c>
+      <c r="C230" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="D230" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="F230" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>991</v>
+      </c>
+      <c r="B231" t="s">
+        <v>977</v>
+      </c>
+      <c r="C231" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="D231" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="F231" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>992</v>
+      </c>
+      <c r="B232" t="s">
+        <v>978</v>
+      </c>
+      <c r="C232" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="D232" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="F232" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>993</v>
+      </c>
+      <c r="B233" t="s">
+        <v>979</v>
+      </c>
+      <c r="C233" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="D233" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="F233" t="s">
+        <v>754</v>
       </c>
     </row>
   </sheetData>

</xml_diff>